<commit_message>
Agregado validación al código de plaza, habilitación del campo cuspp, corrección del mensaje "referencia de objeto no establecida"
</commit_message>
<xml_diff>
--- a/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Formato carga trabajadores.xlsx
+++ b/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Formato carga trabajadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\src\app\00078-GestionPlanillas\WebApp\Assets\application\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA02590-A8D6-4377-8512-B95F030A5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF121669-8810-484E-AD87-8B822BA01284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B84A05A4-1C0C-4BB4-ACF7-40E6BCA93EDC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>nombres</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>codigo_trabajador</t>
+  </si>
+  <si>
+    <t>cuspp</t>
   </si>
 </sst>
 </file>
@@ -477,11 +480,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5930E-3266-41E5-9BCB-BDDEAE3622A2}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -505,11 +506,12 @@
     <col min="18" max="18" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="1"/>
+    <col min="21" max="21" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -571,6 +573,9 @@
         <v>16</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avance carga por lote de trabajadores
</commit_message>
<xml_diff>
--- a/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Formato carga trabajadores.xlsx
+++ b/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Formato carga trabajadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\src\app\00078-GestionPlanillas\WebApp\Assets\application\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF121669-8810-484E-AD87-8B822BA01284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE91DEC-6E82-4F74-8978-EA0D53B2723A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B84A05A4-1C0C-4BB4-ACF7-40E6BCA93EDC}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>dependencia</t>
   </si>
   <si>
-    <t>cuenta_banco</t>
-  </si>
-  <si>
     <t>numero_cuenta</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>cuspp</t>
+  </si>
+  <si>
+    <t>banco</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,35 +488,35 @@
   <cols>
     <col min="1" max="1" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -558,25 +558,25 @@
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó el campo estado a la carga masiva de trabajadores
</commit_message>
<xml_diff>
--- a/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Formato carga trabajadores.xlsx
+++ b/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Formato carga trabajadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\src\app\00078-GestionPlanillas\WebApp\Assets\application\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE91DEC-6E82-4F74-8978-EA0D53B2723A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE6DDA1-EFB2-42FD-99A5-9340E6A7A029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B84A05A4-1C0C-4BB4-ACF7-40E6BCA93EDC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>nombres</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>banco</t>
+  </si>
+  <si>
+    <t>estado</t>
   </si>
 </sst>
 </file>
@@ -480,9 +483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5930E-3266-41E5-9BCB-BDDEAE3622A2}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -511,7 +516,7 @@
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -577,6 +582,9 @@
       </c>
       <c r="V1" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>